<commit_message>
Handle combination of MIP and Balsamic
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.14.mip.xlsx
+++ b/tests/fixtures/orderforms/1508.14.mip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17E4C49-F8B6-6849-9B54-D642970D8EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA80EEF-1A75-CB47-8FD9-FD55552932EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="3640" windowWidth="45800" windowHeight="19700" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="orderform" sheetId="1" r:id="rId2"/>
     <sheet name="Drop down lists" sheetId="6" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="432">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -2768,7 +2771,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3293,6 +3296,34 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3334,38 +3365,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="46" fillId="4" borderId="1" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="323">
@@ -3872,6 +3871,27 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="information"/>
+      <sheetName val="orderform"/>
+      <sheetName val="Drop down lists"/>
+      <sheetName val="Genlista"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4178,7 +4198,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4222,7 +4242,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4565,7 +4585,7 @@
   <dimension ref="A1:AB428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E19" sqref="A9:J19"/>
+      <selection activeCell="T19" sqref="T15:T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -4838,46 +4858,46 @@
       <c r="AB8" s="126"/>
     </row>
     <row r="9" spans="1:28" s="7" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="188" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="182"/>
-      <c r="D9" s="182"/>
-      <c r="E9" s="182"/>
-      <c r="F9" s="182"/>
-      <c r="G9" s="182"/>
-      <c r="H9" s="182"/>
-      <c r="I9" s="182"/>
-      <c r="J9" s="183"/>
+      <c r="B9" s="189"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="189"/>
+      <c r="H9" s="189"/>
+      <c r="I9" s="189"/>
+      <c r="J9" s="190"/>
       <c r="K9" s="63"/>
-      <c r="L9" s="184" t="s">
+      <c r="L9" s="191" t="s">
         <v>106</v>
       </c>
-      <c r="M9" s="185"/>
+      <c r="M9" s="192"/>
       <c r="N9" s="15"/>
-      <c r="O9" s="190" t="s">
+      <c r="O9" s="197" t="s">
         <v>408</v>
       </c>
-      <c r="P9" s="191"/>
-      <c r="Q9" s="191"/>
-      <c r="R9" s="192"/>
+      <c r="P9" s="198"/>
+      <c r="Q9" s="198"/>
+      <c r="R9" s="199"/>
       <c r="S9" s="16"/>
-      <c r="T9" s="186" t="s">
+      <c r="T9" s="193" t="s">
         <v>392</v>
       </c>
-      <c r="U9" s="187"/>
-      <c r="V9" s="188"/>
+      <c r="U9" s="194"/>
+      <c r="V9" s="195"/>
       <c r="W9" s="141"/>
-      <c r="X9" s="193" t="s">
+      <c r="X9" s="200" t="s">
         <v>409</v>
       </c>
-      <c r="Y9" s="194"/>
+      <c r="Y9" s="201"/>
       <c r="Z9" s="16"/>
-      <c r="AA9" s="189" t="s">
+      <c r="AA9" s="196" t="s">
         <v>212</v>
       </c>
-      <c r="AB9" s="189"/>
+      <c r="AB9" s="196"/>
     </row>
     <row r="10" spans="1:28" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A10" s="17" t="s">
@@ -5128,258 +5148,250 @@
       <c r="AB14" s="26"/>
     </row>
     <row r="15" spans="1:28" s="71" customFormat="1" ht="25" customHeight="1">
-      <c r="A15" s="195" t="s">
+      <c r="A15" s="181" t="s">
         <v>420</v>
       </c>
-      <c r="B15" s="196" t="s">
+      <c r="B15" s="182" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="D15" s="197" t="s">
+      <c r="D15" s="183" t="s">
         <v>314</v>
       </c>
-      <c r="E15" s="197" t="s">
+      <c r="E15" s="183" t="s">
         <v>421</v>
       </c>
-      <c r="F15" s="198" t="s">
+      <c r="F15" s="184" t="s">
         <v>422</v>
       </c>
-      <c r="G15" s="199" t="s">
+      <c r="G15" s="185" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="196" t="s">
+      <c r="H15" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="199" t="s">
+      <c r="I15" s="185" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="196" t="s">
+      <c r="J15" s="182" t="s">
         <v>423</v>
       </c>
       <c r="K15" s="67"/>
-      <c r="L15" s="200" t="s">
+      <c r="L15" s="186" t="s">
         <v>424</v>
       </c>
-      <c r="M15" s="196" t="s">
+      <c r="M15" s="182" t="s">
         <v>28</v>
       </c>
       <c r="N15" s="67"/>
-      <c r="O15" s="196" t="s">
+      <c r="O15" s="182" t="s">
         <v>368</v>
       </c>
-      <c r="P15" s="196" t="s">
+      <c r="P15" s="182" t="s">
         <v>425</v>
       </c>
-      <c r="Q15" s="195" t="s">
+      <c r="Q15" s="181" t="s">
         <v>426</v>
       </c>
-      <c r="R15" s="195" t="s">
+      <c r="R15" s="181" t="s">
         <v>427</v>
       </c>
       <c r="S15" s="159"/>
-      <c r="T15" s="201" t="s">
-        <v>95</v>
-      </c>
+      <c r="T15" s="147"/>
       <c r="U15" s="163"/>
       <c r="V15" s="163"/>
       <c r="W15" s="172"/>
       <c r="X15" s="174"/>
       <c r="Y15" s="175"/>
       <c r="Z15" s="69"/>
-      <c r="AA15" s="196">
+      <c r="AA15" s="182">
         <v>220</v>
       </c>
-      <c r="AB15" s="196"/>
+      <c r="AB15" s="182"/>
     </row>
     <row r="16" spans="1:28" s="71" customFormat="1" ht="25" customHeight="1">
-      <c r="A16" s="195" t="s">
+      <c r="A16" s="181" t="s">
         <v>426</v>
       </c>
-      <c r="B16" s="196" t="s">
+      <c r="B16" s="182" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="D16" s="197" t="s">
+      <c r="D16" s="183" t="s">
         <v>314</v>
       </c>
-      <c r="E16" s="197" t="s">
+      <c r="E16" s="183" t="s">
         <v>421</v>
       </c>
-      <c r="F16" s="198" t="s">
+      <c r="F16" s="184" t="s">
         <v>422</v>
       </c>
-      <c r="G16" s="202" t="s">
+      <c r="G16" s="187" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="196" t="s">
+      <c r="H16" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="196" t="s">
+      <c r="I16" s="182" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="196" t="s">
+      <c r="J16" s="182" t="s">
         <v>423</v>
       </c>
       <c r="K16" s="67"/>
-      <c r="L16" s="200" t="s">
+      <c r="L16" s="186" t="s">
         <v>424</v>
       </c>
-      <c r="M16" s="196" t="s">
+      <c r="M16" s="182" t="s">
         <v>29</v>
       </c>
       <c r="N16" s="67"/>
-      <c r="O16" s="196" t="s">
+      <c r="O16" s="182" t="s">
         <v>368</v>
       </c>
-      <c r="P16" s="196" t="s">
+      <c r="P16" s="182" t="s">
         <v>425</v>
       </c>
-      <c r="Q16" s="196"/>
-      <c r="R16" s="196"/>
+      <c r="Q16" s="182"/>
+      <c r="R16" s="182"/>
       <c r="S16" s="159"/>
-      <c r="T16" s="201" t="s">
-        <v>95</v>
-      </c>
+      <c r="T16" s="147"/>
       <c r="U16" s="70"/>
       <c r="V16" s="163"/>
       <c r="W16" s="172"/>
       <c r="X16" s="174"/>
       <c r="Y16" s="175"/>
       <c r="Z16" s="69"/>
-      <c r="AA16" s="196">
+      <c r="AA16" s="182">
         <v>220</v>
       </c>
-      <c r="AB16" s="196" t="s">
+      <c r="AB16" s="182" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:28" s="71" customFormat="1" ht="25" customHeight="1">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="181" t="s">
         <v>427</v>
       </c>
-      <c r="B17" s="196" t="s">
+      <c r="B17" s="182" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="D17" s="197" t="s">
+      <c r="D17" s="183" t="s">
         <v>314</v>
       </c>
-      <c r="E17" s="197" t="s">
+      <c r="E17" s="183" t="s">
         <v>429</v>
       </c>
-      <c r="F17" s="198" t="s">
+      <c r="F17" s="184" t="s">
         <v>422</v>
       </c>
-      <c r="G17" s="202" t="s">
+      <c r="G17" s="187" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="196" t="s">
+      <c r="H17" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="I17" s="196" t="s">
+      <c r="I17" s="182" t="s">
         <v>98</v>
       </c>
-      <c r="J17" s="196" t="s">
+      <c r="J17" s="182" t="s">
         <v>423</v>
       </c>
       <c r="K17" s="67"/>
-      <c r="L17" s="200" t="s">
+      <c r="L17" s="186" t="s">
         <v>424</v>
       </c>
-      <c r="M17" s="196" t="s">
+      <c r="M17" s="182" t="s">
         <v>30</v>
       </c>
       <c r="N17" s="67"/>
-      <c r="O17" s="196" t="s">
+      <c r="O17" s="182" t="s">
         <v>368</v>
       </c>
-      <c r="P17" s="196" t="s">
+      <c r="P17" s="182" t="s">
         <v>425</v>
       </c>
-      <c r="Q17" s="196"/>
-      <c r="R17" s="196"/>
+      <c r="Q17" s="182"/>
+      <c r="R17" s="182"/>
       <c r="S17" s="159"/>
-      <c r="T17" s="201" t="s">
-        <v>95</v>
-      </c>
+      <c r="T17" s="147"/>
       <c r="U17" s="70"/>
       <c r="V17" s="163"/>
       <c r="W17" s="172"/>
       <c r="X17" s="174"/>
       <c r="Y17" s="175"/>
       <c r="Z17" s="69"/>
-      <c r="AA17" s="196">
+      <c r="AA17" s="182">
         <v>220</v>
       </c>
-      <c r="AB17" s="196"/>
+      <c r="AB17" s="182"/>
     </row>
     <row r="18" spans="1:28" s="71" customFormat="1" ht="25" customHeight="1">
-      <c r="A18" s="195" t="s">
+      <c r="A18" s="181" t="s">
         <v>430</v>
       </c>
-      <c r="B18" s="196" t="s">
+      <c r="B18" s="182" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="D18" s="197" t="s">
+      <c r="D18" s="183" t="s">
         <v>314</v>
       </c>
-      <c r="E18" s="197" t="s">
+      <c r="E18" s="183" t="s">
         <v>421</v>
       </c>
-      <c r="F18" s="198" t="s">
+      <c r="F18" s="184" t="s">
         <v>431</v>
       </c>
-      <c r="G18" s="202" t="s">
+      <c r="G18" s="187" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="196" t="s">
+      <c r="H18" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="196" t="s">
+      <c r="I18" s="182" t="s">
         <v>98</v>
       </c>
-      <c r="J18" s="196" t="s">
+      <c r="J18" s="182" t="s">
         <v>423</v>
       </c>
       <c r="K18" s="67"/>
-      <c r="L18" s="200" t="s">
+      <c r="L18" s="186" t="s">
         <v>424</v>
       </c>
-      <c r="M18" s="196" t="s">
+      <c r="M18" s="182" t="s">
         <v>31</v>
       </c>
       <c r="N18" s="67"/>
-      <c r="O18" s="196" t="s">
+      <c r="O18" s="182" t="s">
         <v>368</v>
       </c>
-      <c r="P18" s="196" t="s">
+      <c r="P18" s="182" t="s">
         <v>425</v>
       </c>
-      <c r="Q18" s="196"/>
-      <c r="R18" s="196"/>
+      <c r="Q18" s="182"/>
+      <c r="R18" s="182"/>
       <c r="S18" s="159"/>
-      <c r="T18" s="201" t="s">
-        <v>95</v>
-      </c>
+      <c r="T18" s="147"/>
       <c r="U18" s="70"/>
       <c r="V18" s="163"/>
       <c r="W18" s="172"/>
       <c r="X18" s="174"/>
       <c r="Y18" s="175"/>
       <c r="Z18" s="69"/>
-      <c r="AA18" s="196">
+      <c r="AA18" s="182">
         <v>220</v>
       </c>
-      <c r="AB18" s="196"/>
+      <c r="AB18" s="182"/>
     </row>
     <row r="19" spans="1:28" s="71" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="128"/>
@@ -16487,7 +16499,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="26">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -16552,7 +16564,7 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!$H$3:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T19:T394</xm:sqref>
+          <xm:sqref>T15:T394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
@@ -16574,73 +16586,25 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{0E16313E-A6EB-9146-84F9-F2BA62201FD1}">
           <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
+            <xm:f>'/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/[1508.12.scout.xlsx]Sheet3'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D15:D18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9FBDDE8B-6433-AF40-9AA1-26DE3E5A526D}">
           <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
+            <xm:f>'/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/[1508.12.scout.xlsx]Sheet3'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>I15:I18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)" xr:uid="{D0AD39D1-77EF-BF43-9F18-4C234660D19C}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>T15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This is not a valid input (only yes/no is valid)" xr:uid="{E1BB53B4-AF02-DD47-8B06-5BC64AE16E38}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>T16:T18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{06A501A9-3312-3B4F-8564-58E67F82609D}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>M15:M18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BBA05765-50FB-5A49-93E2-F98D5F005619}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15:B18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61DBDA17-EF28-C74D-AE56-B6BD0E32428D}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E15:E18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95BE239E-5CAE-7A4B-AD9F-73F1EFCE6749}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G15:G18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9307ED0-01B8-C042-B73C-0F85A8CA92F5}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H15:H18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C555BA82-776C-3341-B90C-A12BBB05C1C1}">
-          <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J15:J18</xm:sqref>
+          <xm:sqref>G15:J18 E15:E18 B15:B18 M15:M18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify in the comments collumn if DSD sample!" xr:uid="{9DB61BBB-5E42-3144-949E-7B5447CB57FF}">
           <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Sheet3!#REF!</xm:f>
+            <xm:f>'/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/[1508.12.scout.xlsx]Sheet3'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>P15:P18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{39CD3FAB-1F1C-6F4D-8F31-920B89923CF8}">
           <x14:formula1>
-            <xm:f>[1508.12.scout.xlsx]Genlista!#REF!</xm:f>
+            <xm:f>'/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/[1508.12.scout.xlsx]Genlista'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>O15:O18</xm:sqref>
         </x14:dataValidation>

</xml_diff>